<commit_message>
Version Non fonctionnelle : génération excel
</commit_message>
<xml_diff>
--- a/App_pressing_Loreau/Resources/PatternExcel/LogPattern.xlsx
+++ b/App_pressing_Loreau/Resources/PatternExcel/LogPattern.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700"/>
@@ -15,9 +15,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Nombre de logs</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +62,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,9 +114,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -132,9 +148,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +183,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,38 +359,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
modif d'aurelien sur LogExcel
</commit_message>
<xml_diff>
--- a/App_pressing_Loreau/Resources/PatternExcel/LogPattern.xlsx
+++ b/App_pressing_Loreau/Resources/PatternExcel/LogPattern.xlsx
@@ -16,9 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Nombre de logs</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Nb log</t>
+  </si>
+  <si>
+    <t>message</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,10 +379,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>